<commit_message>
dataProvider and read ExcelDataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/UserData.xlsx
+++ b/src/test/resources/UserData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="113">
   <si>
     <t>Test Case No</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>12/25/1988</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Get a Customized Insurance Quote</t>
   </si>
 </sst>
 </file>
@@ -778,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="21" x14ac:dyDescent="0.55000000000000004"/>
@@ -789,32 +795,33 @@
     <col min="1" max="1" width="14.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="14.140625" style="11"/>
+    <col min="4" max="4" width="33.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="14.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:27" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,76 +832,79 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -904,77 +914,80 @@
       <c r="C2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>25</v>
+      <c r="D2" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -984,77 +997,80 @@
       <c r="C3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>47</v>
+      <c r="D3" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1064,157 +1080,163 @@
       <c r="C4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>56</v>
+      <c r="D4" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V4" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>67</v>
+      <c r="D5" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V5" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA5" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1224,77 +1246,80 @@
       <c r="C6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>76</v>
+      <c r="D6" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V6" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA6" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1302,77 +1327,78 @@
         <v>83</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="R7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="S7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="U7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U7" s="4" t="s">
+      <c r="V7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V7" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1380,155 +1406,157 @@
         <v>66</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="L8" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="R8" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="T8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="U8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U8" s="4" t="s">
+      <c r="V8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V8" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA8" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="O9" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="S9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="V9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V9" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA9" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1536,87 +1564,88 @@
         <v>66</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="S10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="U10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U10" s="4" t="s">
+      <c r="V10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V10" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="W10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA10" s="4" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
-    <hyperlink ref="K2" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
-    <hyperlink ref="K7" r:id="rId6"/>
-    <hyperlink ref="K8" r:id="rId7"/>
-    <hyperlink ref="K9" r:id="rId8"/>
-    <hyperlink ref="K10" r:id="rId9"/>
+    <hyperlink ref="L3" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L5" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L9" r:id="rId8"/>
+    <hyperlink ref="L10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>

</xml_diff>